<commit_message>
Added Display bindings & bug excel macros fix
</commit_message>
<xml_diff>
--- a/Bugs.xlsx
+++ b/Bugs.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18201"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Mark\Documents\TIPPERKIT\APP\"/>
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="171027" iterate="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -23,9 +23,54 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="12">
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>Bug Tracker</t>
+  </si>
+  <si>
+    <t>Priority</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Issue Type</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Updated</t>
+  </si>
+  <si>
+    <t>Title</t>
+  </si>
+  <si>
+    <t>Date Created</t>
+  </si>
+  <si>
+    <t>Not Started</t>
+  </si>
+  <si>
+    <t>Bus1</t>
+  </si>
+  <si>
+    <t>asd</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="dd\-mm\-yy\ hh:mm"/>
+    <numFmt numFmtId="165" formatCode="dd\-mm\-yy\ hh:mm:ss"/>
+  </numFmts>
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -33,16 +78,36 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF242729"/>
+      <name val="Calibri"/>
+      <family val="3"/>
+      <charset val="1"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFEFF0F1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -50,12 +115,173 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -370,14 +596,734 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <sheetPr codeName="Sheet1"/>
+  <dimension ref="B1:I34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="2" width="9.140625" style="17"/>
+    <col min="3" max="3" width="6.42578125" style="17" customWidth="1"/>
+    <col min="4" max="4" width="7.5703125" style="17" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.140625" style="17" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.28515625" style="17" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.140625" style="17" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="27.42578125" style="17" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.140625" style="17" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="17"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:9" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
+    </row>
+    <row r="2" spans="2:9" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="2:9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="8">
+        <v>0</v>
+      </c>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="6" t="str">
+        <f ca="1">IF(C3&lt;&gt;"",IF(G3&lt;&gt;"",G3,NOW()),"")</f>
+        <v/>
+      </c>
+      <c r="H3" s="7" t="str">
+        <f ca="1">IF(E3="", G3, NOW())</f>
+        <v/>
+      </c>
+      <c r="I3" s="9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="2:9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="10">
+        <f ca="1">IF(C4&lt;&gt;"",IF(B4&lt;&gt;"",B4, B3+1),"")</f>
+        <v>1</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" s="2"/>
+      <c r="G4" s="3">
+        <f ca="1">IF(C4&lt;&gt;"",IF(G4&lt;&gt;"",G4,NOW()),"")</f>
+        <v>42921.79761898148</v>
+      </c>
+      <c r="H4" s="19">
+        <f ca="1">IF(E4&lt;&gt;"",IF(H4="",NOW(),H4),"")</f>
+        <v>0</v>
+      </c>
+      <c r="I4" s="11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="2:9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="10" t="str">
+        <f t="shared" ref="B5:B27" si="0">IF(C5&lt;&gt;"",IF(B5&lt;&gt;"",B5, B4+1),"")</f>
+        <v/>
+      </c>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="3" t="str">
+        <f t="shared" ref="G5:G27" ca="1" si="1">IF(C5&lt;&gt;"",IF(G5&lt;&gt;"",G5,NOW()),"")</f>
+        <v/>
+      </c>
+      <c r="H5" s="4"/>
+      <c r="I5" s="11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="2:9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="3" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v/>
+      </c>
+      <c r="H6" s="4"/>
+      <c r="I6" s="11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="2:9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="3" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v/>
+      </c>
+      <c r="H7" s="4"/>
+      <c r="I7" s="11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="2:9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="3" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v/>
+      </c>
+      <c r="H8" s="4" t="str">
+        <f t="shared" ref="H8:H27" ca="1" si="2">IF(E8="", G8, NOW())</f>
+        <v/>
+      </c>
+      <c r="I8" s="11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="2:9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="3" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v/>
+      </c>
+      <c r="H9" s="4" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v/>
+      </c>
+      <c r="I9" s="11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="2:9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="3" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v/>
+      </c>
+      <c r="H10" s="4" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v/>
+      </c>
+      <c r="I10" s="11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="2:9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="3" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v/>
+      </c>
+      <c r="H11" s="4" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v/>
+      </c>
+      <c r="I11" s="11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="2:9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="3" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v/>
+      </c>
+      <c r="H12" s="4" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v/>
+      </c>
+      <c r="I12" s="11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="2:9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="3" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v/>
+      </c>
+      <c r="H13" s="4" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v/>
+      </c>
+      <c r="I13" s="11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="2:9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="3" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v/>
+      </c>
+      <c r="H14" s="4" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v/>
+      </c>
+      <c r="I14" s="11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="2:9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="3" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v/>
+      </c>
+      <c r="H15" s="4" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v/>
+      </c>
+      <c r="I15" s="11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="2:9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="3" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v/>
+      </c>
+      <c r="H16" s="4" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v/>
+      </c>
+      <c r="I16" s="11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="2:9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="3" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v/>
+      </c>
+      <c r="H17" s="4" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v/>
+      </c>
+      <c r="I17" s="11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="18" spans="2:9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="3" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v/>
+      </c>
+      <c r="H18" s="4" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v/>
+      </c>
+      <c r="I18" s="11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="19" spans="2:9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
+      <c r="G19" s="3" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v/>
+      </c>
+      <c r="H19" s="4" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v/>
+      </c>
+      <c r="I19" s="11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="20" spans="2:9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
+      <c r="G20" s="3" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v/>
+      </c>
+      <c r="H20" s="4" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v/>
+      </c>
+      <c r="I20" s="11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="21" spans="2:9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+      <c r="G21" s="3" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v/>
+      </c>
+      <c r="H21" s="4" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v/>
+      </c>
+      <c r="I21" s="11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="22" spans="2:9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="C22" s="2"/>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
+      <c r="G22" s="3" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v/>
+      </c>
+      <c r="H22" s="4" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v/>
+      </c>
+      <c r="I22" s="11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="23" spans="2:9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="C23" s="2"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2"/>
+      <c r="F23" s="2"/>
+      <c r="G23" s="3" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v/>
+      </c>
+      <c r="H23" s="4" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v/>
+      </c>
+      <c r="I23" s="11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="24" spans="2:9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B24" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="C24" s="2"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2"/>
+      <c r="F24" s="2"/>
+      <c r="G24" s="3" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v/>
+      </c>
+      <c r="H24" s="4" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v/>
+      </c>
+      <c r="I24" s="11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="25" spans="2:9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="C25" s="2"/>
+      <c r="D25" s="2"/>
+      <c r="E25" s="2"/>
+      <c r="F25" s="2"/>
+      <c r="G25" s="3" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v/>
+      </c>
+      <c r="H25" s="4" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v/>
+      </c>
+      <c r="I25" s="11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="26" spans="2:9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B26" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="C26" s="2"/>
+      <c r="D26" s="2"/>
+      <c r="E26" s="2"/>
+      <c r="F26" s="2"/>
+      <c r="G26" s="3" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v/>
+      </c>
+      <c r="H26" s="4" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v/>
+      </c>
+      <c r="I26" s="11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="27" spans="2:9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B27" s="12" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="C27" s="13"/>
+      <c r="D27" s="13"/>
+      <c r="E27" s="13"/>
+      <c r="F27" s="13"/>
+      <c r="G27" s="14" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v/>
+      </c>
+      <c r="H27" s="15" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v/>
+      </c>
+      <c r="I27" s="16" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="28" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B28" s="12" t="str">
+        <f t="shared" ref="B28:B34" si="3">IF(C28&lt;&gt;"",IF(B28&lt;&gt;"",B28, B27+1),"")</f>
+        <v/>
+      </c>
+      <c r="C28" s="13"/>
+      <c r="D28" s="13"/>
+      <c r="E28" s="13"/>
+      <c r="F28" s="13"/>
+      <c r="G28" s="14" t="str">
+        <f t="shared" ref="G28:G34" ca="1" si="4">IF(C28&lt;&gt;"",IF(G28&lt;&gt;"",G28,NOW()),"")</f>
+        <v/>
+      </c>
+      <c r="H28" s="15" t="str">
+        <f t="shared" ref="H28:H34" ca="1" si="5">IF(E28="", G28, NOW())</f>
+        <v/>
+      </c>
+      <c r="I28" s="16" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="29" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B29" s="12" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="C29" s="13"/>
+      <c r="D29" s="13"/>
+      <c r="E29" s="13"/>
+      <c r="F29" s="13"/>
+      <c r="G29" s="14" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v/>
+      </c>
+      <c r="H29" s="15" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v/>
+      </c>
+      <c r="I29" s="16" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="30" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B30" s="12" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="C30" s="13"/>
+      <c r="D30" s="13"/>
+      <c r="E30" s="13"/>
+      <c r="F30" s="13"/>
+      <c r="G30" s="14" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v/>
+      </c>
+      <c r="H30" s="15" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v/>
+      </c>
+      <c r="I30" s="16" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="31" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B31" s="12" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="C31" s="13"/>
+      <c r="D31" s="13"/>
+      <c r="E31" s="13"/>
+      <c r="F31" s="13"/>
+      <c r="G31" s="14" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v/>
+      </c>
+      <c r="H31" s="15" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v/>
+      </c>
+      <c r="I31" s="16" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="32" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B32" s="12" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="C32" s="13"/>
+      <c r="D32" s="13"/>
+      <c r="E32" s="13"/>
+      <c r="F32" s="13"/>
+      <c r="G32" s="14" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v/>
+      </c>
+      <c r="H32" s="15" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v/>
+      </c>
+      <c r="I32" s="16" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="33" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B33" s="12" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="C33" s="13"/>
+      <c r="D33" s="13"/>
+      <c r="E33" s="13"/>
+      <c r="F33" s="13"/>
+      <c r="G33" s="14" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v/>
+      </c>
+      <c r="H33" s="15" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v/>
+      </c>
+      <c r="I33" s="16" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="34" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B34" s="12" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="C34" s="13"/>
+      <c r="D34" s="13"/>
+      <c r="E34" s="13"/>
+      <c r="F34" s="13"/>
+      <c r="G34" s="14" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v/>
+      </c>
+      <c r="H34" s="15" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v/>
+      </c>
+      <c r="I34" s="16" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B1:I1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>